<commit_message>
Testing documentation with jupyter notebook
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otavio\Documents\Tech studies\portfolio_python\dataset_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036DE17F-20D6-4DF0-BB82-760E9C19B720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB50CED-B1C4-49E7-8D5C-17E0770804F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Principal" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Principal" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="101">
   <si>
     <t>Posição contratual</t>
   </si>
@@ -305,6 +306,24 @@
   </si>
   <si>
     <t>Maria</t>
+  </si>
+  <si>
+    <t>Natureza do ato</t>
+  </si>
+  <si>
+    <t>Pública</t>
+  </si>
+  <si>
+    <t>Privada</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Miguel</t>
   </si>
 </sst>
 </file>
@@ -363,11 +382,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,15 +725,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585FAB60-F1F0-4E1A-8A68-F026CA504CA4}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.77734375" customWidth="1"/>
     <col min="17" max="17" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5671,26 +5770,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c6dc80bd-117f-42bf-b5e6-e56a26f761da">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="589f4db3-07ba-4e7a-9e14-9dcb48725f20" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F41B1E0CDCE884B80E5B1B509E0F0BA" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f02f5aec8778bfaef68b1b87078fee51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c6dc80bd-117f-42bf-b5e6-e56a26f761da" xmlns:ns3="589f4db3-07ba-4e7a-9e14-9dcb48725f20" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7158d7acffde1d53cf4127c591cb155b" ns2:_="" ns3:_="">
     <xsd:import namespace="c6dc80bd-117f-42bf-b5e6-e56a26f761da"/>
@@ -5909,26 +5988,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E46352C-028E-4028-B21C-EE17F7079752}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c6dc80bd-117f-42bf-b5e6-e56a26f761da"/>
-    <ds:schemaRef ds:uri="589f4db3-07ba-4e7a-9e14-9dcb48725f20"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87921D4F-3BCA-41BA-AD61-7DFB45A1E2BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c6dc80bd-117f-42bf-b5e6-e56a26f761da">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="589f4db3-07ba-4e7a-9e14-9dcb48725f20" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C043D634-D853-4C17-8199-50519FDA4915}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5945,4 +6025,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87921D4F-3BCA-41BA-AD61-7DFB45A1E2BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E46352C-028E-4028-B21C-EE17F7079752}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c6dc80bd-117f-42bf-b5e6-e56a26f761da"/>
+    <ds:schemaRef ds:uri="589f4db3-07ba-4e7a-9e14-9dcb48725f20"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>